<commit_message>
Push the modified POM to GIT
</commit_message>
<xml_diff>
--- a/ProjectUsingPOM/TestData/LoginData.xlsx
+++ b/ProjectUsingPOM/TestData/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANDRASEKHARJANGA\eclipse-workspace\RobotFramework\ProjectUsingPOM\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CHANDRASEKHARJANGA\git\RobotProject\ProjectUsingPOM\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2135AF2A-28FA-4C51-BD00-28AF0EA51609}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0245068B-3EEE-411D-B378-331350608D69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="11964" xr2:uid="{468491BC-B9C9-4F12-AC45-82C45B55A2E4}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>${username}</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>${browser}</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -440,9 +443,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A488FA3-C523-411E-86DB-19B956441447}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -480,11 +485,28 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>